<commit_message>
Various fixes, added solutions, fixed mapping spreadsheet 01
</commit_message>
<xml_diff>
--- a/Master NIEM Document/Mapping_Spreadsheets/01 Native Properties.xlsx
+++ b/Master NIEM Document/Mapping_Spreadsheets/01 Native Properties.xlsx
@@ -591,7 +591,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -610,9 +610,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
@@ -661,10 +658,10 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1802,7 +1799,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:Q24"/>
+  <dimension ref="A2:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
@@ -1815,18 +1812,18 @@
     <col min="3" max="3" width="44.9766" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.35156" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="7" width="32.6719" style="1" customWidth="1"/>
-    <col min="8" max="8" width="32" style="1" customWidth="1"/>
-    <col min="9" max="9" width="23.3516" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="32.6719" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85156" style="1" customWidth="1"/>
-    <col min="13" max="13" width="72.0781" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.1719" style="1" customWidth="1"/>
-    <col min="17" max="17" width="153.672" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.6719" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.3516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="32.6719" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85156" style="1" customWidth="1"/>
+    <col min="12" max="12" width="72.0781" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.1719" style="1" customWidth="1"/>
+    <col min="16" max="16" width="153.672" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -1848,7 +1845,6 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="3">
@@ -1869,713 +1865,690 @@
       <c r="F2" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" t="s" s="4">
+        <v>7</v>
+      </c>
       <c r="H2" t="s" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I2" t="s" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J2" t="s" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K2" t="s" s="4">
-        <v>10</v>
-      </c>
-      <c r="L2" t="s" s="4">
         <v>11</v>
       </c>
-      <c r="M2" t="s" s="5">
+      <c r="L2" t="s" s="5">
         <v>3</v>
       </c>
+      <c r="M2" t="s" s="4">
+        <v>5</v>
+      </c>
       <c r="N2" t="s" s="4">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O2" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="P2" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="Q2" t="s" s="7">
+      <c r="P2" t="s" s="6">
         <v>14</v>
       </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="8">
+      <c r="A3" t="s" s="7">
         <v>15</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" t="s" s="10">
+      <c r="B3" s="8"/>
+      <c r="C3" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="D3" t="s" s="11">
+      <c r="D3" t="s" s="10">
         <v>1</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
       <c r="L3" s="14"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="16"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="15"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="17">
+      <c r="A4" t="s" s="16">
         <v>17</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" t="s" s="19">
+      <c r="B4" s="17"/>
+      <c r="C4" t="s" s="18">
         <v>18</v>
       </c>
-      <c r="D4" t="s" s="20">
+      <c r="D4" t="s" s="19">
         <v>1</v>
       </c>
-      <c r="E4" t="s" s="21">
+      <c r="E4" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F4" t="s" s="22">
+      <c r="F4" t="s" s="21">
         <v>20</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" t="s" s="24">
+      <c r="G4" t="s" s="22">
         <v>21</v>
       </c>
+      <c r="H4" s="23"/>
       <c r="I4" s="23"/>
       <c r="J4" s="23"/>
       <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" t="s" s="25">
+      <c r="L4" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="N4" t="s" s="24">
+      <c r="M4" t="s" s="22">
         <v>19</v>
       </c>
+      <c r="N4" s="23"/>
       <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" t="s" s="26">
+      <c r="P4" t="s" s="25">
         <v>20</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="17">
+      <c r="A5" t="s" s="16">
         <v>17</v>
       </c>
-      <c r="B5" t="s" s="20">
+      <c r="B5" t="s" s="19">
         <v>23</v>
       </c>
-      <c r="C5" t="s" s="19">
+      <c r="C5" t="s" s="18">
         <v>24</v>
       </c>
-      <c r="D5" t="s" s="20">
+      <c r="D5" t="s" s="19">
         <v>25</v>
       </c>
-      <c r="E5" t="s" s="21">
+      <c r="E5" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
       <c r="L5" s="28"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="30"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="29"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="31"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="33"/>
-      <c r="F6" t="s" s="22">
+      <c r="A6" s="30"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="32"/>
+      <c r="F6" t="s" s="21">
         <v>26</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" t="s" s="24">
+      <c r="G6" t="s" s="22">
         <v>27</v>
       </c>
-      <c r="I6" s="23"/>
-      <c r="J6" t="s" s="24">
+      <c r="H6" s="23"/>
+      <c r="I6" t="s" s="22">
         <v>20</v>
       </c>
+      <c r="J6" s="23"/>
       <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" t="s" s="25">
+      <c r="L6" t="s" s="24">
         <v>28</v>
       </c>
-      <c r="N6" t="s" s="24">
+      <c r="M6" t="s" s="22">
         <v>19</v>
       </c>
+      <c r="N6" s="23"/>
       <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" t="s" s="26">
+      <c r="P6" t="s" s="25">
         <v>29</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="17">
+      <c r="A7" t="s" s="16">
         <v>17</v>
       </c>
-      <c r="B7" t="s" s="20">
+      <c r="B7" t="s" s="19">
         <v>30</v>
       </c>
-      <c r="C7" t="s" s="19">
+      <c r="C7" t="s" s="18">
         <v>31</v>
       </c>
-      <c r="D7" t="s" s="20">
+      <c r="D7" t="s" s="19">
         <v>25</v>
       </c>
-      <c r="E7" t="s" s="21">
+      <c r="E7" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F7" t="s" s="22">
+      <c r="F7" t="s" s="21">
         <v>32</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" t="s" s="24">
+      <c r="G7" t="s" s="22">
         <v>33</v>
       </c>
-      <c r="I7" s="23"/>
-      <c r="J7" t="s" s="24">
+      <c r="H7" s="23"/>
+      <c r="I7" t="s" s="22">
         <v>26</v>
       </c>
+      <c r="J7" s="23"/>
       <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" t="s" s="25">
+      <c r="L7" t="s" s="24">
         <v>34</v>
       </c>
-      <c r="N7" t="s" s="24">
+      <c r="M7" t="s" s="22">
         <v>19</v>
       </c>
+      <c r="N7" s="23"/>
       <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" t="s" s="26">
+      <c r="P7" t="s" s="25">
         <v>35</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="17">
+      <c r="A8" t="s" s="16">
         <v>17</v>
       </c>
-      <c r="B8" t="s" s="20">
+      <c r="B8" t="s" s="19">
         <v>36</v>
       </c>
-      <c r="C8" t="s" s="19">
+      <c r="C8" t="s" s="18">
         <v>37</v>
       </c>
-      <c r="D8" t="s" s="20">
+      <c r="D8" t="s" s="19">
         <v>25</v>
       </c>
-      <c r="E8" t="s" s="21">
+      <c r="E8" t="s" s="20">
         <v>38</v>
       </c>
-      <c r="F8" t="s" s="22">
+      <c r="F8" t="s" s="21">
         <v>39</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" t="s" s="24">
+      <c r="G8" t="s" s="22">
         <v>33</v>
       </c>
-      <c r="I8" s="23"/>
-      <c r="J8" t="s" s="24">
+      <c r="H8" s="23"/>
+      <c r="I8" t="s" s="22">
         <v>26</v>
       </c>
+      <c r="J8" s="23"/>
       <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" t="s" s="25">
+      <c r="L8" t="s" s="24">
         <v>40</v>
       </c>
-      <c r="N8" t="s" s="24">
+      <c r="M8" t="s" s="22">
         <v>41</v>
       </c>
+      <c r="N8" s="23"/>
       <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" t="s" s="26">
+      <c r="P8" t="s" s="25">
         <v>42</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="17">
+      <c r="A9" t="s" s="16">
         <v>17</v>
       </c>
-      <c r="B9" t="s" s="20">
+      <c r="B9" t="s" s="19">
         <v>43</v>
       </c>
-      <c r="C9" t="s" s="19">
+      <c r="C9" t="s" s="18">
         <v>44</v>
       </c>
-      <c r="D9" t="s" s="20">
+      <c r="D9" t="s" s="19">
         <v>25</v>
       </c>
-      <c r="E9" t="s" s="21">
+      <c r="E9" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F9" t="s" s="22">
+      <c r="F9" t="s" s="21">
         <v>45</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" t="s" s="24">
+      <c r="G9" t="s" s="22">
         <v>33</v>
       </c>
-      <c r="I9" s="23"/>
-      <c r="J9" t="s" s="24">
+      <c r="H9" s="23"/>
+      <c r="I9" t="s" s="22">
         <v>26</v>
       </c>
+      <c r="J9" s="23"/>
       <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" t="s" s="25">
+      <c r="L9" t="s" s="24">
         <v>46</v>
       </c>
-      <c r="N9" t="s" s="24">
+      <c r="M9" t="s" s="22">
         <v>19</v>
       </c>
+      <c r="N9" s="23"/>
       <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" t="s" s="26">
+      <c r="P9" t="s" s="25">
         <v>47</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="17">
+      <c r="A10" t="s" s="16">
         <v>48</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" t="s" s="19">
+      <c r="B10" s="17"/>
+      <c r="C10" t="s" s="18">
         <v>49</v>
       </c>
-      <c r="D10" t="s" s="20">
+      <c r="D10" t="s" s="19">
         <v>1</v>
       </c>
-      <c r="E10" t="s" s="21">
+      <c r="E10" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
       <c r="L10" s="28"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="30"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="29"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="17">
+      <c r="A11" t="s" s="16">
         <v>48</v>
       </c>
-      <c r="B11" t="s" s="20">
+      <c r="B11" t="s" s="19">
         <v>50</v>
       </c>
-      <c r="C11" t="s" s="19">
+      <c r="C11" t="s" s="18">
         <v>51</v>
       </c>
-      <c r="D11" t="s" s="20">
+      <c r="D11" t="s" s="19">
         <v>25</v>
       </c>
-      <c r="E11" t="s" s="21">
+      <c r="E11" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
       <c r="L11" s="28"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="30"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="29"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="17">
+      <c r="A12" t="s" s="16">
         <v>52</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" t="s" s="19">
+      <c r="B12" s="17"/>
+      <c r="C12" t="s" s="18">
         <v>53</v>
       </c>
-      <c r="D12" t="s" s="20">
+      <c r="D12" t="s" s="19">
         <v>1</v>
       </c>
-      <c r="E12" t="s" s="21">
+      <c r="E12" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
       <c r="L12" s="28"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="30"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="29"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="17">
+      <c r="A13" t="s" s="16">
         <v>52</v>
       </c>
-      <c r="B13" t="s" s="20">
+      <c r="B13" t="s" s="19">
         <v>54</v>
       </c>
-      <c r="C13" t="s" s="19">
+      <c r="C13" t="s" s="18">
         <v>55</v>
       </c>
-      <c r="D13" t="s" s="20">
+      <c r="D13" t="s" s="19">
         <v>25</v>
       </c>
-      <c r="E13" t="s" s="21">
+      <c r="E13" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
       <c r="L13" s="28"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="30"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="29"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="17">
+      <c r="A14" t="s" s="16">
         <v>52</v>
       </c>
-      <c r="B14" t="s" s="20">
+      <c r="B14" t="s" s="19">
         <v>56</v>
       </c>
-      <c r="C14" t="s" s="19">
+      <c r="C14" t="s" s="18">
         <v>57</v>
       </c>
-      <c r="D14" t="s" s="20">
+      <c r="D14" t="s" s="19">
         <v>25</v>
       </c>
-      <c r="E14" t="s" s="21">
+      <c r="E14" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
       <c r="L14" s="28"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="30"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="29"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="17">
+      <c r="A15" t="s" s="16">
         <v>58</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" t="s" s="19">
+      <c r="B15" s="17"/>
+      <c r="C15" t="s" s="18">
         <v>59</v>
       </c>
-      <c r="D15" t="s" s="20">
+      <c r="D15" t="s" s="19">
         <v>1</v>
       </c>
-      <c r="E15" t="s" s="21">
+      <c r="E15" t="s" s="20">
         <v>38</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
       <c r="L15" s="28"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="30"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="29"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="17">
+      <c r="A16" t="s" s="16">
         <v>58</v>
       </c>
-      <c r="B16" t="s" s="20">
+      <c r="B16" t="s" s="19">
         <v>60</v>
       </c>
-      <c r="C16" t="s" s="19">
+      <c r="C16" t="s" s="18">
         <v>61</v>
       </c>
-      <c r="D16" t="s" s="20">
+      <c r="D16" t="s" s="19">
         <v>25</v>
       </c>
-      <c r="E16" t="s" s="21">
+      <c r="E16" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
       <c r="L16" s="28"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="30"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="29"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="17">
+      <c r="A17" t="s" s="16">
         <v>58</v>
       </c>
-      <c r="B17" t="s" s="20">
+      <c r="B17" t="s" s="19">
         <v>62</v>
       </c>
-      <c r="C17" t="s" s="19">
+      <c r="C17" t="s" s="18">
         <v>63</v>
       </c>
-      <c r="D17" t="s" s="20">
+      <c r="D17" t="s" s="19">
         <v>64</v>
       </c>
-      <c r="E17" t="s" s="21">
+      <c r="E17" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
       <c r="L17" s="28"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="30"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="29"/>
     </row>
     <row r="18" ht="32.05" customHeight="1">
-      <c r="A18" t="s" s="17">
+      <c r="A18" t="s" s="16">
         <v>58</v>
       </c>
-      <c r="B18" t="s" s="20">
+      <c r="B18" t="s" s="19">
         <v>65</v>
       </c>
-      <c r="C18" t="s" s="19">
+      <c r="C18" t="s" s="18">
         <v>66</v>
       </c>
-      <c r="D18" t="s" s="20">
+      <c r="D18" t="s" s="19">
         <v>67</v>
       </c>
-      <c r="E18" t="s" s="21">
+      <c r="E18" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
       <c r="L18" s="28"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="30"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="29"/>
     </row>
     <row r="19" ht="32.05" customHeight="1">
-      <c r="A19" t="s" s="17">
+      <c r="A19" t="s" s="16">
         <v>58</v>
       </c>
-      <c r="B19" t="s" s="20">
+      <c r="B19" t="s" s="19">
         <v>68</v>
       </c>
-      <c r="C19" t="s" s="19">
+      <c r="C19" t="s" s="18">
         <v>69</v>
       </c>
-      <c r="D19" t="s" s="20">
+      <c r="D19" t="s" s="19">
         <v>64</v>
       </c>
-      <c r="E19" t="s" s="21">
+      <c r="E19" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
       <c r="L19" s="28"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="30"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="29"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="17">
+      <c r="A20" t="s" s="16">
         <v>48</v>
       </c>
-      <c r="B20" t="s" s="20">
+      <c r="B20" t="s" s="19">
         <v>70</v>
       </c>
-      <c r="C20" t="s" s="19">
+      <c r="C20" t="s" s="18">
         <v>71</v>
       </c>
-      <c r="D20" t="s" s="20">
+      <c r="D20" t="s" s="19">
         <v>25</v>
       </c>
-      <c r="E20" t="s" s="21">
+      <c r="E20" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
       <c r="L20" s="28"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="30"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="29"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="17">
+      <c r="A21" t="s" s="16">
         <v>72</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" t="s" s="19">
+      <c r="B21" s="17"/>
+      <c r="C21" t="s" s="18">
         <v>73</v>
       </c>
-      <c r="D21" t="s" s="20">
+      <c r="D21" t="s" s="19">
         <v>1</v>
       </c>
-      <c r="E21" t="s" s="21">
+      <c r="E21" t="s" s="20">
         <v>74</v>
       </c>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
       <c r="L21" s="28"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="30"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="29"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="17">
+      <c r="A22" t="s" s="16">
         <v>72</v>
       </c>
-      <c r="B22" t="s" s="20">
+      <c r="B22" t="s" s="19">
         <v>75</v>
       </c>
-      <c r="C22" t="s" s="19">
+      <c r="C22" t="s" s="18">
         <v>76</v>
       </c>
-      <c r="D22" t="s" s="20">
+      <c r="D22" t="s" s="19">
         <v>25</v>
       </c>
-      <c r="E22" t="s" s="21">
+      <c r="E22" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
       <c r="L22" s="28"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="30"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="29"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" t="s" s="17">
+      <c r="A23" t="s" s="16">
         <v>72</v>
       </c>
-      <c r="B23" t="s" s="20">
+      <c r="B23" t="s" s="19">
         <v>77</v>
       </c>
-      <c r="C23" t="s" s="19">
+      <c r="C23" t="s" s="18">
         <v>78</v>
       </c>
-      <c r="D23" t="s" s="20">
+      <c r="D23" t="s" s="19">
         <v>67</v>
       </c>
-      <c r="E23" t="s" s="21">
+      <c r="E23" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
       <c r="L23" s="28"/>
-      <c r="M23" s="29"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="28"/>
-      <c r="Q23" s="30"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="29"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="34">
+      <c r="A24" t="s" s="33">
         <v>72</v>
       </c>
-      <c r="B24" t="s" s="35">
+      <c r="B24" t="s" s="34">
         <v>79</v>
       </c>
-      <c r="C24" t="s" s="36">
+      <c r="C24" t="s" s="35">
         <v>80</v>
       </c>
-      <c r="D24" t="s" s="35">
+      <c r="D24" t="s" s="34">
         <v>67</v>
       </c>
-      <c r="E24" t="s" s="37">
+      <c r="E24" t="s" s="36">
         <v>19</v>
       </c>
-      <c r="F24" s="38"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
       <c r="L24" s="39"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="39"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="39"/>
-      <c r="Q24" s="41"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>